<commit_message>
order placement sceanrio for oxo us
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/OXO/GoldOxoTestData1.xlsx
+++ b/src/test/resources/TestData/OXO/GoldOxoTestData1.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02DCD8D6-31F0-4651-A638-DD4E6FE7E5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B5C0FC-E98D-495D-B991-A78A541F9346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="order_Placement" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>03/30</t>
   </si>
   <si>
-    <t>Ground</t>
-  </si>
-  <si>
     <t>United State</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>AccountDetails25</t>
+  </si>
+  <si>
+    <t>Ground Shipping</t>
   </si>
 </sst>
 </file>
@@ -586,53 +586,53 @@
   <dimension ref="A1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="56.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="56.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.44140625" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="30.5546875" customWidth="1"/>
-    <col min="12" max="12" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5546875" customWidth="1"/>
-    <col min="14" max="14" width="24.44140625" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" customWidth="1"/>
-    <col min="16" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="30.5703125" customWidth="1"/>
+    <col min="12" max="12" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="24.42578125" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="11" customWidth="1"/>
     <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="14" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="19.44140625" customWidth="1"/>
-    <col min="30" max="30" width="40.44140625" customWidth="1"/>
+    <col min="26" max="26" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="19.42578125" customWidth="1"/>
+    <col min="30" max="30" width="40.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>2</v>
@@ -641,22 +641,22 @@
         <v>3</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>14</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>4</v>
@@ -680,10 +680,10 @@
         <v>7</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>8</v>
@@ -698,48 +698,48 @@
         <v>10</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AC1" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="AI1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
         <v>15</v>
@@ -748,27 +748,27 @@
         <v>16</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O2" t="s">
         <v>17</v>
       </c>
       <c r="P2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q2" t="s">
         <v>19</v>
@@ -783,7 +783,7 @@
         <v>9898989898</v>
       </c>
       <c r="V2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>20</v>
@@ -795,21 +795,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>15</v>
@@ -818,27 +818,27 @@
         <v>16</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O3" t="s">
         <v>17</v>
       </c>
       <c r="P3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q3" t="s">
         <v>19</v>
@@ -853,7 +853,7 @@
         <v>9898989898</v>
       </c>
       <c r="V3" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>20</v>
@@ -865,21 +865,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
         <v>15</v>
@@ -888,27 +888,27 @@
         <v>16</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4">
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O4" t="s">
         <v>17</v>
       </c>
       <c r="P4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q4" t="s">
         <v>19</v>
@@ -923,7 +923,7 @@
         <v>9898989898</v>
       </c>
       <c r="V4" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X4" s="3" t="s">
         <v>20</v>
@@ -935,21 +935,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
         <v>15</v>
@@ -958,27 +958,27 @@
         <v>16</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5">
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O5" t="s">
         <v>17</v>
       </c>
       <c r="P5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q5" t="s">
         <v>19</v>
@@ -993,7 +993,7 @@
         <v>9898989898</v>
       </c>
       <c r="V5" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>20</v>
@@ -1005,21 +1005,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" t="s">
         <v>15</v>
@@ -1028,27 +1028,27 @@
         <v>16</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M6">
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O6" t="s">
         <v>17</v>
       </c>
       <c r="P6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q6" t="s">
         <v>19</v>
@@ -1063,7 +1063,7 @@
         <v>9898989898</v>
       </c>
       <c r="V6" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X6" s="3" t="s">
         <v>20</v>
@@ -1075,21 +1075,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>15</v>
@@ -1098,27 +1098,27 @@
         <v>16</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M7">
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O7" t="s">
         <v>17</v>
       </c>
       <c r="P7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q7" t="s">
         <v>19</v>
@@ -1133,7 +1133,7 @@
         <v>9898989898</v>
       </c>
       <c r="V7" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X7" s="3" t="s">
         <v>20</v>
@@ -1145,21 +1145,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -1168,27 +1168,27 @@
         <v>16</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="N8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O8" t="s">
         <v>17</v>
       </c>
       <c r="P8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q8" t="s">
         <v>19</v>
@@ -1203,7 +1203,7 @@
         <v>9898989898</v>
       </c>
       <c r="V8" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X8" s="3" t="s">
         <v>20</v>
@@ -1215,21 +1215,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
@@ -1238,27 +1238,27 @@
         <v>16</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="N9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O9" t="s">
         <v>17</v>
       </c>
       <c r="P9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q9" t="s">
         <v>19</v>
@@ -1273,7 +1273,7 @@
         <v>9898989898</v>
       </c>
       <c r="V9" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>20</v>
@@ -1285,21 +1285,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
@@ -1308,27 +1308,27 @@
         <v>16</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
       <c r="N10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O10" t="s">
         <v>17</v>
       </c>
       <c r="P10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q10" t="s">
         <v>19</v>
@@ -1343,7 +1343,7 @@
         <v>9898989898</v>
       </c>
       <c r="V10" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X10" s="3" t="s">
         <v>20</v>
@@ -1355,21 +1355,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
         <v>15</v>
@@ -1378,27 +1378,27 @@
         <v>16</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M11">
         <v>1</v>
       </c>
       <c r="N11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O11" t="s">
         <v>17</v>
       </c>
       <c r="P11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q11" t="s">
         <v>19</v>
@@ -1413,7 +1413,7 @@
         <v>9898989898</v>
       </c>
       <c r="V11" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>20</v>
@@ -1425,21 +1425,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -1448,27 +1448,27 @@
         <v>16</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M12">
         <v>1</v>
       </c>
       <c r="N12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O12" t="s">
         <v>17</v>
       </c>
       <c r="P12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q12" t="s">
         <v>19</v>
@@ -1483,7 +1483,7 @@
         <v>9898989898</v>
       </c>
       <c r="V12" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X12" s="3" t="s">
         <v>20</v>
@@ -1495,21 +1495,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
@@ -1518,27 +1518,27 @@
         <v>16</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M13">
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O13" t="s">
         <v>17</v>
       </c>
       <c r="P13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q13" t="s">
         <v>19</v>
@@ -1553,7 +1553,7 @@
         <v>9898989898</v>
       </c>
       <c r="V13" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>20</v>
@@ -1565,21 +1565,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s">
         <v>15</v>
@@ -1588,27 +1588,27 @@
         <v>16</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I14" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M14">
         <v>1</v>
       </c>
       <c r="N14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O14" t="s">
         <v>17</v>
       </c>
       <c r="P14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q14" t="s">
         <v>19</v>
@@ -1623,7 +1623,7 @@
         <v>9898989898</v>
       </c>
       <c r="V14" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X14" s="3" t="s">
         <v>20</v>
@@ -1635,21 +1635,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
         <v>15</v>
@@ -1658,27 +1658,27 @@
         <v>16</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M15">
         <v>1</v>
       </c>
       <c r="N15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O15" t="s">
         <v>17</v>
       </c>
       <c r="P15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q15" t="s">
         <v>19</v>
@@ -1693,7 +1693,7 @@
         <v>9898989898</v>
       </c>
       <c r="V15" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X15" s="3" t="s">
         <v>20</v>
@@ -1705,21 +1705,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" t="s">
         <v>15</v>
@@ -1728,27 +1728,27 @@
         <v>16</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M16">
         <v>1</v>
       </c>
       <c r="N16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O16" t="s">
         <v>17</v>
       </c>
       <c r="P16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q16" t="s">
         <v>19</v>
@@ -1763,7 +1763,7 @@
         <v>9898989898</v>
       </c>
       <c r="V16" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X16" s="3" t="s">
         <v>20</v>
@@ -1775,21 +1775,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" t="s">
         <v>15</v>
@@ -1798,27 +1798,27 @@
         <v>16</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M17">
         <v>1</v>
       </c>
       <c r="N17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O17" t="s">
         <v>17</v>
       </c>
       <c r="P17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q17" t="s">
         <v>19</v>
@@ -1833,7 +1833,7 @@
         <v>9898989898</v>
       </c>
       <c r="V17" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X17" s="3" t="s">
         <v>20</v>
@@ -1845,21 +1845,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
         <v>15</v>
@@ -1868,27 +1868,27 @@
         <v>16</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M18">
         <v>1</v>
       </c>
       <c r="N18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O18" t="s">
         <v>17</v>
       </c>
       <c r="P18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q18" t="s">
         <v>19</v>
@@ -1903,7 +1903,7 @@
         <v>9898989898</v>
       </c>
       <c r="V18" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X18" s="3" t="s">
         <v>20</v>
@@ -1915,21 +1915,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F19" t="s">
         <v>15</v>
@@ -1938,27 +1938,27 @@
         <v>16</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M19">
         <v>1</v>
       </c>
       <c r="N19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O19" t="s">
         <v>17</v>
       </c>
       <c r="P19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q19" t="s">
         <v>19</v>
@@ -1973,7 +1973,7 @@
         <v>9898989898</v>
       </c>
       <c r="V19" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X19" s="3" t="s">
         <v>20</v>
@@ -1985,21 +1985,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" t="s">
         <v>15</v>
@@ -2008,27 +2008,27 @@
         <v>16</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M20">
         <v>1</v>
       </c>
       <c r="N20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O20" t="s">
         <v>17</v>
       </c>
       <c r="P20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q20" t="s">
         <v>19</v>
@@ -2043,7 +2043,7 @@
         <v>9898989898</v>
       </c>
       <c r="V20" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X20" s="3" t="s">
         <v>20</v>
@@ -2055,21 +2055,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F21" t="s">
         <v>15</v>
@@ -2078,27 +2078,27 @@
         <v>16</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M21">
         <v>1</v>
       </c>
       <c r="N21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O21" t="s">
         <v>17</v>
       </c>
       <c r="P21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q21" t="s">
         <v>19</v>
@@ -2113,7 +2113,7 @@
         <v>9898989898</v>
       </c>
       <c r="V21" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>20</v>
@@ -2125,21 +2125,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F22" t="s">
         <v>15</v>
@@ -2148,27 +2148,27 @@
         <v>16</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M22">
         <v>1</v>
       </c>
       <c r="N22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O22" t="s">
         <v>17</v>
       </c>
       <c r="P22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q22" t="s">
         <v>19</v>
@@ -2183,7 +2183,7 @@
         <v>9898989898</v>
       </c>
       <c r="V22" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X22" s="3" t="s">
         <v>20</v>
@@ -2195,21 +2195,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F23" t="s">
         <v>15</v>
@@ -2218,27 +2218,27 @@
         <v>16</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M23">
         <v>1</v>
       </c>
       <c r="N23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O23" t="s">
         <v>17</v>
       </c>
       <c r="P23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q23" t="s">
         <v>19</v>
@@ -2253,7 +2253,7 @@
         <v>9898989898</v>
       </c>
       <c r="V23" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X23" s="3" t="s">
         <v>20</v>
@@ -2265,21 +2265,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" t="s">
         <v>15</v>
@@ -2288,27 +2288,27 @@
         <v>16</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M24">
         <v>1</v>
       </c>
       <c r="N24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O24" t="s">
         <v>17</v>
       </c>
       <c r="P24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q24" t="s">
         <v>19</v>
@@ -2323,7 +2323,7 @@
         <v>9898989898</v>
       </c>
       <c r="V24" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X24" s="3" t="s">
         <v>20</v>
@@ -2335,21 +2335,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" t="s">
         <v>15</v>
@@ -2358,27 +2358,27 @@
         <v>16</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M25">
         <v>1</v>
       </c>
       <c r="N25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O25" t="s">
         <v>17</v>
       </c>
       <c r="P25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q25" t="s">
         <v>19</v>
@@ -2393,7 +2393,7 @@
         <v>9898989898</v>
       </c>
       <c r="V25" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X25" s="3" t="s">
         <v>20</v>
@@ -2405,21 +2405,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
         <v>15</v>
@@ -2428,27 +2428,27 @@
         <v>16</v>
       </c>
       <c r="H26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M26">
         <v>1</v>
       </c>
       <c r="N26" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O26" t="s">
         <v>17</v>
       </c>
       <c r="P26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q26" t="s">
         <v>19</v>
@@ -2463,7 +2463,7 @@
         <v>9898989898</v>
       </c>
       <c r="V26" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X26" s="3" t="s">
         <v>20</v>
@@ -2475,21 +2475,21 @@
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
@@ -2498,27 +2498,27 @@
         <v>16</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M27">
         <v>1</v>
       </c>
       <c r="N27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O27" t="s">
         <v>17</v>
       </c>
       <c r="P27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Q27" t="s">
         <v>19</v>
@@ -2533,7 +2533,7 @@
         <v>9898989898</v>
       </c>
       <c r="V27" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="X27" s="3" t="s">
         <v>20</v>

</xml_diff>